<commit_message>
object per scanline counter
</commit_message>
<xml_diff>
--- a/References/RAM.xlsx
+++ b/References/RAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelle\Documents\GitHub\FlanSparx\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EB181-4D5E-48D3-B656-19DA0FD8FE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1AFBEE-B3CA-4DDC-AC4C-ACE30281F0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="126">
   <si>
     <t>C000</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Total memory:</t>
+  </si>
+  <si>
+    <t>FFB0</t>
+  </si>
+  <si>
+    <t>curr_enemy_count</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0\ &quot;bytes&quot;"/>
+    <numFmt numFmtId="164" formatCode="0\ &quot;bytes&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -443,7 +449,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,8 +764,8 @@
         <v>4672</v>
       </c>
       <c r="G2" s="1">
-        <f>SUM(L7:L999)</f>
-        <v>56</v>
+        <f>SUM(L7:L1000)</f>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -772,7 +778,7 @@
       </c>
       <c r="G3" s="1">
         <f>G4-G2</f>
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -836,7 +842,7 @@
         <v>26</v>
       </c>
       <c r="K7" t="str">
-        <f>DEC2HEX(HEX2DEC(J7)+L7-1)</f>
+        <f t="shared" ref="K7:K44" si="0">DEC2HEX(HEX2DEC(J7)+L7-1)</f>
         <v>FF87</v>
       </c>
       <c r="L7">
@@ -864,7 +870,7 @@
         <v>42</v>
       </c>
       <c r="K8" t="str">
-        <f>DEC2HEX(HEX2DEC(J8)+L8-1)</f>
+        <f t="shared" si="0"/>
         <v>FF88</v>
       </c>
       <c r="L8">
@@ -892,7 +898,7 @@
         <v>43</v>
       </c>
       <c r="K9" t="str">
-        <f>DEC2HEX(HEX2DEC(J9)+L9-1)</f>
+        <f t="shared" si="0"/>
         <v>FF89</v>
       </c>
       <c r="L9">
@@ -920,7 +926,7 @@
         <v>44</v>
       </c>
       <c r="K10" t="str">
-        <f>DEC2HEX(HEX2DEC(J10)+L10-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8A</v>
       </c>
       <c r="L10">
@@ -944,7 +950,7 @@
         <v>45</v>
       </c>
       <c r="K11" t="str">
-        <f>DEC2HEX(HEX2DEC(J11)+L11-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8B</v>
       </c>
       <c r="L11">
@@ -972,7 +978,7 @@
         <v>46</v>
       </c>
       <c r="K12" t="str">
-        <f>DEC2HEX(HEX2DEC(J12)+L12-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8C</v>
       </c>
       <c r="L12">
@@ -996,7 +1002,7 @@
         <v>47</v>
       </c>
       <c r="K13" t="str">
-        <f>DEC2HEX(HEX2DEC(J13)+L13-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8D</v>
       </c>
       <c r="L13">
@@ -1024,7 +1030,7 @@
         <v>48</v>
       </c>
       <c r="K14" t="str">
-        <f>DEC2HEX(HEX2DEC(J14)+L14-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8E</v>
       </c>
       <c r="L14">
@@ -1053,7 +1059,7 @@
         <v>49</v>
       </c>
       <c r="K15" t="str">
-        <f>DEC2HEX(HEX2DEC(J15)+L15-1)</f>
+        <f t="shared" si="0"/>
         <v>FF8F</v>
       </c>
       <c r="L15">
@@ -1068,7 +1074,7 @@
         <v>50</v>
       </c>
       <c r="K16" t="str">
-        <f>DEC2HEX(HEX2DEC(J16)+L16-1)</f>
+        <f t="shared" si="0"/>
         <v>FF90</v>
       </c>
       <c r="L16">
@@ -1083,7 +1089,7 @@
         <v>51</v>
       </c>
       <c r="K17" t="str">
-        <f>DEC2HEX(HEX2DEC(J17)+L17-1)</f>
+        <f t="shared" si="0"/>
         <v>FF91</v>
       </c>
       <c r="L17">
@@ -1098,7 +1104,7 @@
         <v>52</v>
       </c>
       <c r="K18" t="str">
-        <f>DEC2HEX(HEX2DEC(J18)+L18-1)</f>
+        <f t="shared" si="0"/>
         <v>FF92</v>
       </c>
       <c r="L18">
@@ -1113,7 +1119,7 @@
         <v>53</v>
       </c>
       <c r="K19" t="str">
-        <f>DEC2HEX(HEX2DEC(J19)+L19-1)</f>
+        <f t="shared" si="0"/>
         <v>FF93</v>
       </c>
       <c r="L19">
@@ -1128,7 +1134,7 @@
         <v>54</v>
       </c>
       <c r="K20" t="str">
-        <f>DEC2HEX(HEX2DEC(J20)+L20-1)</f>
+        <f t="shared" si="0"/>
         <v>FF94</v>
       </c>
       <c r="L20">
@@ -1143,7 +1149,7 @@
         <v>55</v>
       </c>
       <c r="K21" t="str">
-        <f>DEC2HEX(HEX2DEC(J21)+L21-1)</f>
+        <f t="shared" si="0"/>
         <v>FF95</v>
       </c>
       <c r="L21">
@@ -1158,7 +1164,7 @@
         <v>56</v>
       </c>
       <c r="K22" t="str">
-        <f>DEC2HEX(HEX2DEC(J22)+L22-1)</f>
+        <f t="shared" si="0"/>
         <v>FF96</v>
       </c>
       <c r="L22">
@@ -1173,7 +1179,7 @@
         <v>57</v>
       </c>
       <c r="K23" t="str">
-        <f>DEC2HEX(HEX2DEC(J23)+L23-1)</f>
+        <f t="shared" si="0"/>
         <v>FF97</v>
       </c>
       <c r="L23">
@@ -1188,7 +1194,7 @@
         <v>58</v>
       </c>
       <c r="K24" t="str">
-        <f>DEC2HEX(HEX2DEC(J24)+L24-1)</f>
+        <f t="shared" si="0"/>
         <v>FF98</v>
       </c>
       <c r="L24">
@@ -1203,7 +1209,7 @@
         <v>59</v>
       </c>
       <c r="K25" t="str">
-        <f>DEC2HEX(HEX2DEC(J25)+L25-1)</f>
+        <f t="shared" si="0"/>
         <v>FF99</v>
       </c>
       <c r="L25">
@@ -1218,7 +1224,7 @@
         <v>60</v>
       </c>
       <c r="K26" t="str">
-        <f>DEC2HEX(HEX2DEC(J26)+L26-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9A</v>
       </c>
       <c r="L26">
@@ -1233,7 +1239,7 @@
         <v>61</v>
       </c>
       <c r="K27" t="str">
-        <f>DEC2HEX(HEX2DEC(J27)+L27-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9B</v>
       </c>
       <c r="L27">
@@ -1248,7 +1254,7 @@
         <v>79</v>
       </c>
       <c r="K28" t="str">
-        <f>DEC2HEX(HEX2DEC(J28)+L28-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9C</v>
       </c>
       <c r="L28">
@@ -1263,7 +1269,7 @@
         <v>80</v>
       </c>
       <c r="K29" t="str">
-        <f>DEC2HEX(HEX2DEC(J29)+L29-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9D</v>
       </c>
       <c r="L29">
@@ -1278,7 +1284,7 @@
         <v>81</v>
       </c>
       <c r="K30" t="str">
-        <f>DEC2HEX(HEX2DEC(J30)+L30-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9E</v>
       </c>
       <c r="L30">
@@ -1293,7 +1299,7 @@
         <v>82</v>
       </c>
       <c r="K31" t="str">
-        <f>DEC2HEX(HEX2DEC(J31)+L31-1)</f>
+        <f t="shared" si="0"/>
         <v>FF9F</v>
       </c>
       <c r="L31">
@@ -1308,7 +1314,7 @@
         <v>83</v>
       </c>
       <c r="K32" t="str">
-        <f>DEC2HEX(HEX2DEC(J32)+L32-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA0</v>
       </c>
       <c r="L32">
@@ -1323,7 +1329,7 @@
         <v>84</v>
       </c>
       <c r="K33" t="str">
-        <f>DEC2HEX(HEX2DEC(J33)+L33-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA1</v>
       </c>
       <c r="L33">
@@ -1338,7 +1344,7 @@
         <v>85</v>
       </c>
       <c r="K34" t="str">
-        <f>DEC2HEX(HEX2DEC(J34)+L34-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA2</v>
       </c>
       <c r="L34">
@@ -1353,7 +1359,7 @@
         <v>86</v>
       </c>
       <c r="K35" t="str">
-        <f>DEC2HEX(HEX2DEC(J35)+L35-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA3</v>
       </c>
       <c r="L35">
@@ -1368,7 +1374,7 @@
         <v>87</v>
       </c>
       <c r="K36" t="str">
-        <f>DEC2HEX(HEX2DEC(J36)+L36-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA4</v>
       </c>
       <c r="L36">
@@ -1383,7 +1389,7 @@
         <v>88</v>
       </c>
       <c r="K37" t="str">
-        <f>DEC2HEX(HEX2DEC(J37)+L37-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA5</v>
       </c>
       <c r="L37">
@@ -1398,7 +1404,7 @@
         <v>89</v>
       </c>
       <c r="K38" t="str">
-        <f>DEC2HEX(HEX2DEC(J38)+L38-1)</f>
+        <f t="shared" si="0"/>
         <v>FFA9</v>
       </c>
       <c r="L38">
@@ -1413,7 +1419,7 @@
         <v>90</v>
       </c>
       <c r="K39" t="str">
-        <f>DEC2HEX(HEX2DEC(J39)+L39-1)</f>
+        <f t="shared" si="0"/>
         <v>FFAA</v>
       </c>
       <c r="L39">
@@ -1428,7 +1434,7 @@
         <v>96</v>
       </c>
       <c r="K40" t="str">
-        <f>DEC2HEX(HEX2DEC(J40)+L40-1)</f>
+        <f t="shared" si="0"/>
         <v>FFAB</v>
       </c>
       <c r="L40">
@@ -1443,7 +1449,7 @@
         <v>97</v>
       </c>
       <c r="K41" t="str">
-        <f>DEC2HEX(HEX2DEC(J41)+L41-1)</f>
+        <f t="shared" si="0"/>
         <v>FFAC</v>
       </c>
       <c r="L41">
@@ -1458,7 +1464,7 @@
         <v>98</v>
       </c>
       <c r="K42" t="str">
-        <f>DEC2HEX(HEX2DEC(J42)+L42-1)</f>
+        <f t="shared" si="0"/>
         <v>FFAD</v>
       </c>
       <c r="L42">
@@ -1473,7 +1479,7 @@
         <v>99</v>
       </c>
       <c r="K43" t="str">
-        <f>DEC2HEX(HEX2DEC(J43)+L43-1)</f>
+        <f t="shared" si="0"/>
         <v>FFAE</v>
       </c>
       <c r="L43">
@@ -1487,156 +1493,171 @@
       <c r="J44" t="s">
         <v>100</v>
       </c>
-      <c r="K44" t="s">
-        <v>101</v>
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>FFAF</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J45" t="s">
-        <v>102</v>
-      </c>
-      <c r="K45" t="str">
-        <f>DEC2HEX(HEX2DEC(J45)+L45-1)</f>
-        <v>FFF0</v>
-      </c>
-      <c r="L45">
-        <v>1</v>
+        <v>124</v>
+      </c>
+      <c r="K45" t="s">
+        <v>101</v>
       </c>
       <c r="M45" t="s">
-        <v>112</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K46" t="str">
-        <f>DEC2HEX(HEX2DEC(J46)+L46-1)</f>
-        <v>FFF1</v>
+        <f t="shared" ref="K46:K54" si="1">DEC2HEX(HEX2DEC(J46)+L46-1)</f>
+        <v>FFF0</v>
       </c>
       <c r="L46">
         <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K47" t="str">
-        <f>DEC2HEX(HEX2DEC(J47)+L47-1)</f>
-        <v>FFF2</v>
+        <f t="shared" si="1"/>
+        <v>FFF1</v>
       </c>
       <c r="L47">
         <v>1</v>
       </c>
       <c r="M47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K48" t="str">
-        <f>DEC2HEX(HEX2DEC(J48)+L48-1)</f>
-        <v>FFF3</v>
+        <f t="shared" si="1"/>
+        <v>FFF2</v>
       </c>
       <c r="L48">
         <v>1</v>
       </c>
       <c r="M48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K49" t="str">
-        <f>DEC2HEX(HEX2DEC(J49)+L49-1)</f>
-        <v>FFF4</v>
+        <f t="shared" si="1"/>
+        <v>FFF3</v>
       </c>
       <c r="L49">
         <v>1</v>
       </c>
       <c r="M49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K50" t="str">
-        <f>DEC2HEX(HEX2DEC(J50)+L50-1)</f>
-        <v>FFF5</v>
+        <f t="shared" si="1"/>
+        <v>FFF4</v>
       </c>
       <c r="L50">
         <v>1</v>
       </c>
       <c r="M50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K51" t="str">
-        <f>DEC2HEX(HEX2DEC(J51)+L51-1)</f>
-        <v>FFF6</v>
+        <f t="shared" si="1"/>
+        <v>FFF5</v>
       </c>
       <c r="L51">
         <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K52" t="str">
-        <f>DEC2HEX(HEX2DEC(J52)+L52-1)</f>
-        <v>FFF7</v>
+        <f t="shared" si="1"/>
+        <v>FFF6</v>
       </c>
       <c r="L52">
         <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K53" t="str">
-        <f>DEC2HEX(HEX2DEC(J53)+L53-1)</f>
-        <v>FFF8</v>
+        <f t="shared" si="1"/>
+        <v>FFF7</v>
       </c>
       <c r="L53">
         <v>1</v>
       </c>
       <c r="M53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="10:13" x14ac:dyDescent="0.3">
       <c r="J54" t="s">
+        <v>110</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="1"/>
+        <v>FFF8</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="J55" t="s">
         <v>111</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K55" t="s">
         <v>121</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M55" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>